<commit_message>
- Add content type as optional parameter - Add tests for non text responses
</commit_message>
<xml_diff>
--- a/src/main/resources/side_by_side_tests.xlsx
+++ b/src/main/resources/side_by_side_tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="0" windowWidth="16800" windowHeight="21000"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="38400" windowHeight="21600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Search All Records</t>
   </si>
@@ -45,19 +45,55 @@
   </si>
   <si>
     <t>q=lsid%3Aurn%3Alsid%3Abiodiversity.org.au%3Aafd.taxon%3Ab1d9bf29-648f-47e6-8544-2c2fbdf632b1&amp;facets=genus</t>
+  </si>
+  <si>
+    <t>Mapping legend search macropus</t>
+  </si>
+  <si>
+    <t>q=macropus&amp;cm=species&amp;type=application/json</t>
+  </si>
+  <si>
+    <t>mapping/legend</t>
+  </si>
+  <si>
+    <t>Generate static map</t>
+  </si>
+  <si>
+    <t>pcolour=3531FF&amp;popacity=1&amp;outlineColour=0x000000&amp;dpi=300&amp;scale=on&amp;format=jpg&amp;outline=true&amp;q=Macropus+rufus&amp;extents=96.173828125,-47.11468820158343,169.826171875,-2.5694811631203973&amp;baselayer=world&amp;fileName=MyMap.jpg&amp;pradiusmm=1</t>
+  </si>
+  <si>
+    <t>mapping/wms/image</t>
+  </si>
+  <si>
+    <t>application/json</t>
+  </si>
+  <si>
+    <t>application/octet-stream</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF6A8759"/>
+      <name val="Monaco"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,8 +116,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,50 +434,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="85.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" customWidth="1"/>
+    <col min="1" max="1" width="124.6640625" customWidth="1"/>
+    <col min="2" max="2" width="85.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Adding more tests to sydebyside testing. - Adding hardcoded (but commented) values for easy testing within the IDE
</commit_message>
<xml_diff>
--- a/src/main/resources/side_by_side_tests.xlsx
+++ b/src/main/resources/side_by_side_tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="38400" windowHeight="21600"/>
+    <workbookView xWindow="6200" yWindow="7620" windowWidth="38400" windowHeight="21600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Search All Records</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>application/octet-stream</t>
+  </si>
+  <si>
+    <t>Search for Raw/Provided Scientific Name 'Acacia dealbata' should turn up assorted silver wattles</t>
+  </si>
+  <si>
+    <t>q=raw_name%3A%22Acacia%20dealbata%22&amp;start=0&amp;pageSize=20&amp;sort=first_loaded_date&amp;dir=desc&amp;qc=&amp;facets=taxon_name</t>
+  </si>
+  <si>
+    <t>Search for Raw/Provided Scientific Name 'Osphranter rufus' should turn up assorted red kangaroos</t>
+  </si>
+  <si>
+    <t>q=raw_name%3A%22Osphranter%20rufus%22&amp;start=0&amp;pageSize=20&amp;sort=first_loaded_date&amp;dir=desc&amp;qc=&amp;facets=taxon_name</t>
   </si>
 </sst>
 </file>
@@ -434,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,30 +497,54 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Search for species group Mammals should not have any weird kingdoms, phyla or classes floating about
</commit_message>
<xml_diff>
--- a/src/main/resources/side_by_side_tests.xlsx
+++ b/src/main/resources/side_by_side_tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Search All Records</t>
   </si>
@@ -81,13 +81,30 @@
   </si>
   <si>
     <t>q=raw_name%3A%22Osphranter%20rufus%22&amp;start=0&amp;pageSize=20&amp;sort=first_loaded_date&amp;dir=desc&amp;qc=&amp;facets=taxon_name</t>
+  </si>
+  <si>
+    <r>
+      <t>Search for species group </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>Mammals</t>
+    </r>
+  </si>
+  <si>
+    <t>q=species_group%3AMammals&amp;start=0&amp;pageSize=20&amp;sort=first_loaded_date&amp;dir=desc&amp;qc=&amp;facets=class&amp;facets=phylum&amp;facets=kingdom&amp;flimit=10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -96,15 +113,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF6A8759"/>
-      <name val="Monaco"/>
+      <sz val="14"/>
+      <color rgb="FF24292E"/>
+      <name val="Consolas"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -128,10 +139,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,16 +455,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="124.6640625" customWidth="1"/>
-    <col min="2" max="2" width="85.6640625" customWidth="1"/>
+    <col min="2" max="2" width="60.1640625" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="27.83203125" customWidth="1"/>
   </cols>
@@ -464,7 +473,6 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
       <c r="C1" t="s">
         <v>5</v>
       </c>
@@ -476,7 +484,6 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2"/>
       <c r="C2" t="s">
         <v>5</v>
       </c>
@@ -488,7 +495,6 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2"/>
       <c r="C3" t="s">
         <v>5</v>
       </c>
@@ -497,54 +503,63 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2"/>
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2"/>
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Expanding list of enpoints for side by side tests spreadsheet.
</commit_message>
<xml_diff>
--- a/src/main/resources/side_by_side_tests.xlsx
+++ b/src/main/resources/side_by_side_tests.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mol109/IdeaProjects/biocache-tests/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0E967C52-3B04-AC47-B3E0-E793216CB1A9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6200" yWindow="7620" windowWidth="38400" windowHeight="21600"/>
+    <workbookView xWindow="19900" yWindow="12960" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="66">
   <si>
     <t>Search All Records</t>
   </si>
@@ -99,12 +102,147 @@
   <si>
     <t>q=species_group%3AMammals&amp;start=0&amp;pageSize=20&amp;sort=first_loaded_date&amp;dir=desc&amp;qc=&amp;facets=class&amp;facets=phylum&amp;facets=kingdom&amp;flimit=10</t>
   </si>
+  <si>
+    <t>Listing of layers for taxa in the genus Macropus</t>
+  </si>
+  <si>
+    <t>Static map for the red kangaroo</t>
+  </si>
+  <si>
+    <t>Shape File Download for genus Macropus agilis</t>
+  </si>
+  <si>
+    <t>Disable Record Issues in download</t>
+  </si>
+  <si>
+    <t>BOLD - Australia breakdown</t>
+  </si>
+  <si>
+    <t>An example showing 2 layers for 2 separate species overlaid on the same map using leafletjs.</t>
+  </si>
+  <si>
+    <t>Download all Acacia abbatiana records  with all the default fields and all record issues specifying a "testing" reason for the download.</t>
+  </si>
+  <si>
+    <t>ogc/ows</t>
+  </si>
+  <si>
+    <t>q=genus:Macropus</t>
+  </si>
+  <si>
+    <t>q=Macropus+rufus</t>
+  </si>
+  <si>
+    <t>density/map</t>
+  </si>
+  <si>
+    <t>q=Acacia+abbatiana&amp;reasonTypeId=10</t>
+  </si>
+  <si>
+    <t>occurrences/index/download</t>
+  </si>
+  <si>
+    <t>q=Macropus+agilis&amp;reasonTypeId=10&amp;fileType=shp</t>
+  </si>
+  <si>
+    <t>q=genus:Dugong&amp;reasonTypeId=10&amp;qa=none</t>
+  </si>
+  <si>
+    <t>rank=phylum</t>
+  </si>
+  <si>
+    <t>breakdown/dataResources/dr375</t>
+  </si>
+  <si>
+    <t>ogc/wms/reflect</t>
+  </si>
+  <si>
+    <t>text/plain</t>
+  </si>
+  <si>
+    <t>Download Macropus rufus static map</t>
+  </si>
+  <si>
+    <t>Download E.gunnii lats and longs</t>
+  </si>
+  <si>
+    <t>Find species of Macropus that have an invalid collection date (An example of using assertions to filter taxa)</t>
+  </si>
+  <si>
+    <t>pradiusmm=1&amp;extents=96.173828125,-47.11468820158343,169.826171875,-2.5694811631203973&amp;scale=on&amp;outline=true&amp;fileName=MyMap.jpg&amp;pcolour=3531FF&amp;outlineColour=0x000000&amp;q=Macropus+rufus&amp;dpi=300&amp;format=jpg&amp;baselayer=world&amp;popacity=1</t>
+  </si>
+  <si>
+    <t>reasonTypeId=10&amp;fq=basis_of_record:LivingSpecimen&amp;qa=none&amp;fields=latitude,longitude&amp;q=Eucalyptus+gunnii</t>
+  </si>
+  <si>
+    <t>pageSize=0&amp;fq=assertions:invalidCollectionDate&amp;q=genus:Macropus</t>
+  </si>
+  <si>
+    <t>Assertion code listing (List the assertion codes with categories)</t>
+  </si>
+  <si>
+    <t>Retrieve a count of species in Birds Australia (Retrieve a count of species in Birds Australia and return the first 100)</t>
+  </si>
+  <si>
+    <t>Example climate watch record (Example climate watch record full details)</t>
+  </si>
+  <si>
+    <t>Scatterplot example (Example for Macropus Rufus and environmental layers Temperature - annual mean (Bio01) and Precipitation - annual (bio12))</t>
+  </si>
+  <si>
+    <t>Species legend for macropus. (Legend for WMS q=macropus with cm=species as JSON.)</t>
+  </si>
+  <si>
+    <t>Search for eucalyptus gunnii (Default search)</t>
+  </si>
+  <si>
+    <t>eucalyptus gunnii (Exclude synonyms)</t>
+  </si>
+  <si>
+    <t>Search for eucalyptus (Show occurrence counts for NSW only)</t>
+  </si>
+  <si>
+    <t>Search for eucalyptus gunnii (Include matches with 0 occurrences)</t>
+  </si>
+  <si>
+    <t>assertions/codes</t>
+  </si>
+  <si>
+    <t>facets=taxon_name&amp;flimit=100&amp;q=data_resource_uid:dr359</t>
+  </si>
+  <si>
+    <t>occurrence/facets</t>
+  </si>
+  <si>
+    <t>occurrences/794e1d5b-fc14-4b77-a21a-8e73749dc910</t>
+  </si>
+  <si>
+    <t>q=Macropus%20Agilis&amp;y=el893&amp;x=el874&amp;pointradius=2&amp;height=512&amp;pointcolour=FF0000&amp;width=512</t>
+  </si>
+  <si>
+    <t>scatterplot</t>
+  </si>
+  <si>
+    <t>autocomplete/search</t>
+  </si>
+  <si>
+    <t>q=eucalyptus&amp;fq=cl927%3A%22New+South+Wales+%28including+Coastal+Waters%29%22</t>
+  </si>
+  <si>
+    <t>q=eucalyptus+gunnii</t>
+  </si>
+  <si>
+    <t>synonyms=false&amp;q=eucalyptus+gunnii</t>
+  </si>
+  <si>
+    <t>q=eucalyptus+gunnii&amp;all=true</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -117,6 +255,14 @@
       <color rgb="FF24292E"/>
       <name val="Consolas"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,13 +282,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -454,11 +603,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,8 +712,549 @@
         <v>11</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D9" r:id="rId1" display="http://biocache.ala.org.au/ws/?q=genus:Macropus" xr:uid="{ECE119E9-5AB6-3640-9448-29D81267D848}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244224B7-2F7F-1C45-A668-4892B4EC3B09}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A1:D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="100.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="222.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D9" r:id="rId1" display="http://biocache.ala.org.au/ws/?q=genus:Macropus" xr:uid="{D11023AD-2031-AD49-AE96-0E72F6FE4B4F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Fixing tests where comparisson is not feasible WIP
</commit_message>
<xml_diff>
--- a/src/main/resources/side_by_side_tests.xlsx
+++ b/src/main/resources/side_by_side_tests.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mol109/IdeaProjects/biocache-tests/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0E967C52-3B04-AC47-B3E0-E793216CB1A9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0FEDDAFB-9251-B84D-9274-A204EF715093}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19900" yWindow="12960" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="340" yWindow="6740" windowWidth="29100" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="64">
   <si>
     <t>Search All Records</t>
   </si>
@@ -175,18 +174,12 @@
     <t>reasonTypeId=10&amp;fq=basis_of_record:LivingSpecimen&amp;qa=none&amp;fields=latitude,longitude&amp;q=Eucalyptus+gunnii</t>
   </si>
   <si>
-    <t>pageSize=0&amp;fq=assertions:invalidCollectionDate&amp;q=genus:Macropus</t>
-  </si>
-  <si>
     <t>Assertion code listing (List the assertion codes with categories)</t>
   </si>
   <si>
     <t>Retrieve a count of species in Birds Australia (Retrieve a count of species in Birds Australia and return the first 100)</t>
   </si>
   <si>
-    <t>Example climate watch record (Example climate watch record full details)</t>
-  </si>
-  <si>
     <t>Scatterplot example (Example for Macropus Rufus and environmental layers Temperature - annual mean (Bio01) and Precipitation - annual (bio12))</t>
   </si>
   <si>
@@ -214,9 +207,6 @@
     <t>occurrence/facets</t>
   </si>
   <si>
-    <t>occurrences/794e1d5b-fc14-4b77-a21a-8e73749dc910</t>
-  </si>
-  <si>
     <t>q=Macropus%20Agilis&amp;y=el893&amp;x=el874&amp;pointradius=2&amp;height=512&amp;pointcolour=FF0000&amp;width=512</t>
   </si>
   <si>
@@ -236,6 +226,9 @@
   </si>
   <si>
     <t>q=eucalyptus+gunnii&amp;all=true</t>
+  </si>
+  <si>
+    <t>pageSize=0&amp;fq=assertions:invalidCollectionDate&amp;q=genus:Macropus&amp;facets=taxon_name</t>
   </si>
 </sst>
 </file>
@@ -604,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection sqref="A1:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -823,108 +816,100 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" t="s">
         <v>61</v>
-      </c>
-      <c r="D24" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" t="s">
-        <v>65</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" display="http://biocache.ala.org.au/ws/?q=genus:Macropus" xr:uid="{ECE119E9-5AB6-3640-9448-29D81267D848}"/>
+    <hyperlink ref="D9" r:id="rId1" display="http://biocache.ala.org.au/ws/?q=genus:Macropus" xr:uid="{95053486-EAAE-7745-BE90-EDACC76BCFEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -933,10 +918,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244224B7-2F7F-1C45-A668-4892B4EC3B09}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A1:D27"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A1:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1152,108 +1137,100 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" t="s">
         <v>61</v>
-      </c>
-      <c r="D24" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" t="s">
-        <v>65</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" display="http://biocache.ala.org.au/ws/?q=genus:Macropus" xr:uid="{D11023AD-2031-AD49-AE96-0E72F6FE4B4F}"/>
+    <hyperlink ref="D9" r:id="rId1" display="http://biocache.ala.org.au/ws/?q=genus:Macropus" xr:uid="{C2BD5DD6-5EFD-3241-8244-77CEEC9A95D2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- Tests with binary output were moved to AssortedServicesTest and more detailed checks were added.
</commit_message>
<xml_diff>
--- a/src/main/resources/side_by_side_tests.xlsx
+++ b/src/main/resources/side_by_side_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mol109/IdeaProjects/biocache-tests/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0FEDDAFB-9251-B84D-9274-A204EF715093}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9179531A-2337-304C-81DA-5AC8682B432D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="6740" windowWidth="29100" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="21600" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="64">
   <si>
     <t>Search All Records</t>
   </si>
@@ -597,17 +597,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="124.6640625" customWidth="1"/>
     <col min="2" max="2" width="60.1640625" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -721,189 +721,109 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" t="s">
         <v>58</v>
       </c>
-      <c r="D23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="D19" t="s">
         <v>62</v>
       </c>
     </row>
@@ -918,10 +838,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244224B7-2F7F-1C45-A668-4892B4EC3B09}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A1:D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1100,131 +1020,122 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
         <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
         <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
         <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1233,5 +1144,6 @@
     <hyperlink ref="D9" r:id="rId1" display="http://biocache.ala.org.au/ws/?q=genus:Macropus" xr:uid="{C2BD5DD6-5EFD-3241-8244-77CEEC9A95D2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>